<commit_message>
5paisa working market orders
</commit_message>
<xml_diff>
--- a/config/MirrorTradesystem.xlsx
+++ b/config/MirrorTradesystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debashis\Documents\GitHub\ruby-mirror-trading\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B147AEB-0407-4AE4-8B92-AEA14784577B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E488A522-A5E3-44E9-A26A-67591137F8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>PrimaryAcc</t>
   </si>
@@ -44,89 +36,77 @@
     <t>YES</t>
   </si>
   <si>
-    <t>API Key</t>
-  </si>
-  <si>
-    <t>Api Secret</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>Access Token</t>
   </si>
   <si>
-    <t>GenerateRequestToken</t>
-  </si>
-  <si>
     <t>Client Name</t>
   </si>
   <si>
-    <t>Client ID</t>
-  </si>
-  <si>
-    <t>Request Token</t>
-  </si>
-  <si>
     <t>ON</t>
   </si>
   <si>
     <t>Dynamic Lot size</t>
   </si>
   <si>
-    <t>Broker</t>
-  </si>
-  <si>
-    <t>Angel</t>
-  </si>
-  <si>
-    <t>Zerodha</t>
-  </si>
-  <si>
     <t>Algo Switch</t>
   </si>
   <si>
     <t>Allow Trade</t>
   </si>
   <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>efgh</t>
-  </si>
-  <si>
-    <t>ijkl</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>DEF</t>
-  </si>
-  <si>
-    <t>IJK</t>
-  </si>
-  <si>
-    <t>asdadasdasd</t>
-  </si>
-  <si>
-    <t>asdadasdaasdad</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Fyer</t>
+    <t>User Key</t>
+  </si>
+  <si>
+    <t>Encryption Secret</t>
+  </si>
+  <si>
+    <t>UseriD</t>
+  </si>
+  <si>
+    <t>TOTP</t>
+  </si>
+  <si>
+    <t>MPIN</t>
+  </si>
+  <si>
+    <t>App Source</t>
+  </si>
+  <si>
+    <t>Client Code</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Carlos Guevera</t>
+  </si>
+  <si>
+    <t>abcdefgh</t>
+  </si>
+  <si>
+    <t>bcdefghi</t>
+  </si>
+  <si>
+    <t>asdadasdaddaadasda</t>
+  </si>
+  <si>
+    <t>adadaddaadaaddsada</t>
+  </si>
+  <si>
+    <t>asdasdas</t>
+  </si>
+  <si>
+    <t>adaadasd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,14 +137,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF3F3F3F"/>
@@ -177,12 +149,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -221,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -296,42 +262,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -341,44 +310,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -575,19 +513,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A3:J6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Input">
-  <autoFilter ref="A3:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Client ID" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Client Name" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="API Key" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Api Secret" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="GenerateRequestToken" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Request Token" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Access Token" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity Multiplier" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Allow Trade" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D10439A3-76A4-4DBD-A2C2-AE9F2FB69166}" name="Broker" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A3:K5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" headerRowCellStyle="Input">
+  <autoFilter ref="A3:K5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Client Code" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Client Name" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="User Key" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Encryption Secret" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{66470A22-A1A3-4E16-87F1-98A07A50B9B2}" name="App Source"/>
+    <tableColumn id="12" xr3:uid="{5E64549E-8890-4921-98BC-406C204FD449}" name="TOTP"/>
+    <tableColumn id="13" xr3:uid="{A11046E4-8C7A-4417-8454-BDF24F71FBB1}" name="MPIN"/>
+    <tableColumn id="10" xr3:uid="{781D2363-94CD-4FC7-9FA3-99F0392A6D1F}" name="UseriD"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Access Token" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity Multiplier" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Allow Trade" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -890,189 +829,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="23" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+    <col min="9" max="9" width="31.44140625" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>53570093</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>1231231</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>12345</v>
+      </c>
+      <c r="G4">
+        <v>123456</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>123132131</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>23456</v>
+      </c>
+      <c r="G5">
+        <v>123456</v>
+      </c>
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="J5" s="4">
         <v>2</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="K5" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:J2"/>
+    <mergeCell ref="D1:K2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ON,OFF"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{9F4CDF09-7621-4B52-8D73-7620402E079C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>